<commit_message>
Excel Columns rows 170-224
</commit_message>
<xml_diff>
--- a/brfss_dataset/Columns.xlsx
+++ b/brfss_dataset/Columns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/I516258/Documents/GitHub/data-mining-project/brfss_dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulh\PycharmProjects\data-mining-project\brfss_dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEA2647-931A-E84C-B5EE-1EA699E9C64D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D80F75-AA02-4345-A198-A9A40B0BB1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="19860" xr2:uid="{FF219293-3088-A942-AB16-D1D3DC90A824}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{FF219293-3088-A942-AB16-D1D3DC90A824}"/>
   </bookViews>
   <sheets>
     <sheet name="All columns" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="577">
   <si>
     <t>relevant</t>
   </si>
@@ -1601,6 +1601,177 @@
   </si>
   <si>
     <t>take aspirin to reduce chance of stroke</t>
+  </si>
+  <si>
+    <t>describe arthritis today</t>
+  </si>
+  <si>
+    <t>doctor suggest loosing weight - arthritis</t>
+  </si>
+  <si>
+    <t>doctor suggest physical activity -arthritis</t>
+  </si>
+  <si>
+    <t>taken educational course - arthritis</t>
+  </si>
+  <si>
+    <t>tetanus shot</t>
+  </si>
+  <si>
+    <t>hpv vaccination</t>
+  </si>
+  <si>
+    <t>how many hpv shots</t>
+  </si>
+  <si>
+    <t>shingles/zoster vaccine</t>
+  </si>
+  <si>
+    <t>mammogram - x-ray for breast cancer</t>
+  </si>
+  <si>
+    <t>how long since last mammogram</t>
+  </si>
+  <si>
+    <t>Pap test - cervix cancer</t>
+  </si>
+  <si>
+    <t>how long since last pap test</t>
+  </si>
+  <si>
+    <t>HPV test</t>
+  </si>
+  <si>
+    <t>last HPV test</t>
+  </si>
+  <si>
+    <t>ever had hysterectomy - remove womb</t>
+  </si>
+  <si>
+    <t>ever had clinical breast exam</t>
+  </si>
+  <si>
+    <t>how long since last breast exam</t>
+  </si>
+  <si>
+    <t>blood stool test</t>
+  </si>
+  <si>
+    <t>how long since last blood stool test</t>
+  </si>
+  <si>
+    <t>Sigmoidoscopy and colonoscopy - sign for cancer</t>
+  </si>
+  <si>
+    <t>MOST RECENT exam a sigmoidoscopy or a colonoscopy</t>
+  </si>
+  <si>
+    <t>long since  last sigmoidoscopy or colonoscopy</t>
+  </si>
+  <si>
+    <t>talked about advantages of PSA test</t>
+  </si>
+  <si>
+    <t>disadvantages of the PSA test</t>
+  </si>
+  <si>
+    <t>recommended that you have a PSA test</t>
+  </si>
+  <si>
+    <t>ever had a PSA test</t>
+  </si>
+  <si>
+    <t>How long since last PSA test</t>
+  </si>
+  <si>
+    <t>main reason for psa test</t>
+  </si>
+  <si>
+    <t>decision to have psa test</t>
+  </si>
+  <si>
+    <t>who decided</t>
+  </si>
+  <si>
+    <t>stress about paying rent</t>
+  </si>
+  <si>
+    <t>worried about buying nutritious meals</t>
+  </si>
+  <si>
+    <t>kind of payment at work (hour/job/salary)</t>
+  </si>
+  <si>
+    <t>working hours</t>
+  </si>
+  <si>
+    <t>last kind of payment</t>
+  </si>
+  <si>
+    <t>working hours a week</t>
+  </si>
+  <si>
+    <t>sexual orientation</t>
+  </si>
+  <si>
+    <t>transgender</t>
+  </si>
+  <si>
+    <t>gender of child</t>
+  </si>
+  <si>
+    <t>relation to child</t>
+  </si>
+  <si>
+    <t>doctor said child has asthma</t>
+  </si>
+  <si>
+    <t>still asthma</t>
+  </si>
+  <si>
+    <t>how often get social/emotional support</t>
+  </si>
+  <si>
+    <t>life satisfaction</t>
+  </si>
+  <si>
+    <t>litlle interest/pleasure in doing things</t>
+  </si>
+  <si>
+    <t>feeloing down/depressed/hopeless</t>
+  </si>
+  <si>
+    <t>trouble falling asleep</t>
+  </si>
+  <si>
+    <t>felt tired or little energy</t>
+  </si>
+  <si>
+    <t>poor appetite/eaten too much</t>
+  </si>
+  <si>
+    <t>felt bad about yourself letting someone down</t>
+  </si>
+  <si>
+    <t>trouble concentrating</t>
+  </si>
+  <si>
+    <t>being slow or fast</t>
+  </si>
+  <si>
+    <t>taking medicine for mental health</t>
+  </si>
+  <si>
+    <t>doctor diagnosed anxiety</t>
+  </si>
+  <si>
+    <t>sexual orientation not related</t>
+  </si>
+  <si>
+    <t>gender not related</t>
+  </si>
+  <si>
+    <t>relationship not important</t>
   </si>
 </sst>
 </file>
@@ -1965,11 +2136,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7A19900-7E7D-8F4B-BF9A-701FBC80E4D0}">
   <dimension ref="A1:F331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="E165" sqref="E165"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A181" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A276" sqref="A276"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="2" max="2" width="38.6640625" customWidth="1"/>
@@ -1978,7 +2150,7 @@
     <col min="5" max="5" width="45.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>396</v>
       </c>
@@ -1992,7 +2164,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>81</v>
       </c>
@@ -2006,7 +2178,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -2023,7 +2195,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -2036,7 +2208,7 @@
       </c>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -2049,7 +2221,7 @@
       </c>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>85</v>
       </c>
@@ -2062,7 +2234,7 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>86</v>
       </c>
@@ -2075,7 +2247,7 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>87</v>
       </c>
@@ -2088,7 +2260,7 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>88</v>
       </c>
@@ -2101,7 +2273,7 @@
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>89</v>
       </c>
@@ -2114,7 +2286,7 @@
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -2127,7 +2299,7 @@
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -2140,7 +2312,7 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>92</v>
       </c>
@@ -2153,7 +2325,7 @@
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>93</v>
       </c>
@@ -2166,7 +2338,7 @@
       </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>94</v>
       </c>
@@ -2179,7 +2351,7 @@
       </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>95</v>
       </c>
@@ -2192,7 +2364,7 @@
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>96</v>
       </c>
@@ -2205,7 +2377,7 @@
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>97</v>
       </c>
@@ -2218,7 +2390,7 @@
       </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>98</v>
       </c>
@@ -2231,7 +2403,7 @@
       </c>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>99</v>
       </c>
@@ -2244,7 +2416,7 @@
       </c>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>100</v>
       </c>
@@ -2257,7 +2429,7 @@
       </c>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>101</v>
       </c>
@@ -2270,7 +2442,7 @@
       </c>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>102</v>
       </c>
@@ -2283,7 +2455,7 @@
       </c>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>103</v>
       </c>
@@ -2296,7 +2468,7 @@
       </c>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>104</v>
       </c>
@@ -2309,7 +2481,7 @@
       </c>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>105</v>
       </c>
@@ -2322,7 +2494,7 @@
       </c>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>106</v>
       </c>
@@ -2335,7 +2507,7 @@
       </c>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -2349,7 +2521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -2363,7 +2535,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2377,7 +2549,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>107</v>
       </c>
@@ -2394,7 +2566,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -2408,7 +2580,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>108</v>
       </c>
@@ -2422,7 +2594,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -2436,7 +2608,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -2450,7 +2622,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -2464,7 +2636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>109</v>
       </c>
@@ -2478,7 +2650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>110</v>
       </c>
@@ -2495,7 +2667,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>111</v>
       </c>
@@ -2512,7 +2684,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -2526,7 +2698,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -2540,7 +2712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -2554,7 +2726,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -2568,7 +2740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -2582,7 +2754,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>112</v>
       </c>
@@ -2596,7 +2768,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>113</v>
       </c>
@@ -2613,7 +2785,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>114</v>
       </c>
@@ -2628,7 +2800,7 @@
       </c>
       <c r="E47" s="5"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>115</v>
       </c>
@@ -2643,7 +2815,7 @@
       </c>
       <c r="E48" s="5"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>51</v>
       </c>
@@ -2657,7 +2829,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>116</v>
       </c>
@@ -2677,7 +2849,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -2691,7 +2863,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>53</v>
       </c>
@@ -2705,7 +2877,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>117</v>
       </c>
@@ -2725,7 +2897,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -2739,7 +2911,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>118</v>
       </c>
@@ -2753,7 +2925,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2770,7 +2942,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>119</v>
       </c>
@@ -2784,7 +2956,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>120</v>
       </c>
@@ -2801,7 +2973,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>121</v>
       </c>
@@ -2814,7 +2986,7 @@
       </c>
       <c r="E59" s="5"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>122</v>
       </c>
@@ -2827,7 +2999,7 @@
       </c>
       <c r="E60" s="5"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>123</v>
       </c>
@@ -2841,7 +3013,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>56</v>
       </c>
@@ -2858,7 +3030,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>124</v>
       </c>
@@ -2872,7 +3044,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>57</v>
       </c>
@@ -2886,7 +3058,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>125</v>
       </c>
@@ -2903,7 +3075,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>126</v>
       </c>
@@ -2920,7 +3092,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>127</v>
       </c>
@@ -2937,7 +3109,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>128</v>
       </c>
@@ -2954,7 +3126,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>129</v>
       </c>
@@ -2971,7 +3143,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>130</v>
       </c>
@@ -2988,7 +3160,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>131</v>
       </c>
@@ -3002,7 +3174,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>132</v>
       </c>
@@ -3019,7 +3191,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>133</v>
       </c>
@@ -3033,7 +3205,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>134</v>
       </c>
@@ -3047,7 +3219,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>135</v>
       </c>
@@ -3061,7 +3233,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>58</v>
       </c>
@@ -3078,7 +3250,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>59</v>
       </c>
@@ -3091,7 +3263,7 @@
       </c>
       <c r="E77" s="5"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>136</v>
       </c>
@@ -3104,7 +3276,7 @@
       </c>
       <c r="E78" s="5"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>137</v>
       </c>
@@ -3117,7 +3289,7 @@
       </c>
       <c r="E79" s="5"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>138</v>
       </c>
@@ -3130,7 +3302,7 @@
       </c>
       <c r="E80" s="5"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>60</v>
       </c>
@@ -3147,7 +3319,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>139</v>
       </c>
@@ -3160,7 +3332,7 @@
       </c>
       <c r="E82" s="5"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>140</v>
       </c>
@@ -3173,7 +3345,7 @@
       </c>
       <c r="E83" s="5"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>141</v>
       </c>
@@ -3186,7 +3358,7 @@
       </c>
       <c r="E84" s="5"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>142</v>
       </c>
@@ -3203,7 +3375,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>143</v>
       </c>
@@ -3216,7 +3388,7 @@
       </c>
       <c r="E86" s="5"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>144</v>
       </c>
@@ -3229,7 +3401,7 @@
       </c>
       <c r="E87" s="5"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>145</v>
       </c>
@@ -3242,7 +3414,7 @@
       </c>
       <c r="E88" s="5"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>146</v>
       </c>
@@ -3255,7 +3427,7 @@
       </c>
       <c r="E89" s="5"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>147</v>
       </c>
@@ -3268,7 +3440,7 @@
       </c>
       <c r="E90" s="5"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>61</v>
       </c>
@@ -3285,7 +3457,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>62</v>
       </c>
@@ -3298,7 +3470,7 @@
       </c>
       <c r="E92" s="5"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>148</v>
       </c>
@@ -3311,7 +3483,7 @@
       </c>
       <c r="E93" s="5"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>149</v>
       </c>
@@ -3324,7 +3496,7 @@
       </c>
       <c r="E94" s="5"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>150</v>
       </c>
@@ -3337,7 +3509,7 @@
       </c>
       <c r="E95" s="5"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>151</v>
       </c>
@@ -3350,7 +3522,7 @@
       </c>
       <c r="E96" s="5"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>152</v>
       </c>
@@ -3363,7 +3535,7 @@
       </c>
       <c r="E97" s="5"/>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>63</v>
       </c>
@@ -3380,7 +3552,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>153</v>
       </c>
@@ -3397,7 +3569,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>154</v>
       </c>
@@ -3410,7 +3582,7 @@
       </c>
       <c r="E100" s="5"/>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>155</v>
       </c>
@@ -3423,7 +3595,7 @@
       </c>
       <c r="E101" s="5"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>156</v>
       </c>
@@ -3437,7 +3609,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>157</v>
       </c>
@@ -3451,7 +3623,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>158</v>
       </c>
@@ -3465,7 +3637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>159</v>
       </c>
@@ -3482,7 +3654,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>160</v>
       </c>
@@ -3496,7 +3668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>161</v>
       </c>
@@ -3510,7 +3682,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>162</v>
       </c>
@@ -3524,7 +3696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>163</v>
       </c>
@@ -3541,7 +3713,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>164</v>
       </c>
@@ -3554,7 +3726,7 @@
       </c>
       <c r="E110" s="5"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>165</v>
       </c>
@@ -3568,7 +3740,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>166</v>
       </c>
@@ -3582,7 +3754,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>167</v>
       </c>
@@ -3596,7 +3768,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>168</v>
       </c>
@@ -3610,7 +3782,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>169</v>
       </c>
@@ -3624,7 +3796,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>170</v>
       </c>
@@ -3638,7 +3810,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>171</v>
       </c>
@@ -3652,7 +3824,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>172</v>
       </c>
@@ -3666,7 +3838,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>173</v>
       </c>
@@ -3680,7 +3852,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>174</v>
       </c>
@@ -3694,7 +3866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>175</v>
       </c>
@@ -3708,7 +3880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>176</v>
       </c>
@@ -3722,7 +3894,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>177</v>
       </c>
@@ -3736,7 +3908,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>178</v>
       </c>
@@ -3750,7 +3922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>179</v>
       </c>
@@ -3764,7 +3936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>180</v>
       </c>
@@ -3778,7 +3950,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>181</v>
       </c>
@@ -3795,7 +3967,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>182</v>
       </c>
@@ -3810,7 +3982,7 @@
       </c>
       <c r="E128" s="5"/>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>183</v>
       </c>
@@ -3825,7 +3997,7 @@
       </c>
       <c r="E129" s="5"/>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>184</v>
       </c>
@@ -3840,7 +4012,7 @@
       </c>
       <c r="E130" s="5"/>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>185</v>
       </c>
@@ -3855,7 +4027,7 @@
       </c>
       <c r="E131" s="5"/>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>186</v>
       </c>
@@ -3870,7 +4042,7 @@
       </c>
       <c r="E132" s="5"/>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>187</v>
       </c>
@@ -3885,7 +4057,7 @@
       </c>
       <c r="E133" s="5"/>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>188</v>
       </c>
@@ -3900,7 +4072,7 @@
       </c>
       <c r="E134" s="5"/>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>189</v>
       </c>
@@ -3914,7 +4086,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>190</v>
       </c>
@@ -3928,7 +4100,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>191</v>
       </c>
@@ -3942,7 +4114,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>192</v>
       </c>
@@ -3956,7 +4128,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>193</v>
       </c>
@@ -3970,7 +4142,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>194</v>
       </c>
@@ -3984,7 +4156,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>195</v>
       </c>
@@ -3998,7 +4170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>196</v>
       </c>
@@ -4012,7 +4184,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>197</v>
       </c>
@@ -4026,7 +4198,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>198</v>
       </c>
@@ -4040,7 +4212,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>199</v>
       </c>
@@ -4054,7 +4226,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>200</v>
       </c>
@@ -4068,7 +4240,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>201</v>
       </c>
@@ -4085,7 +4257,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>202</v>
       </c>
@@ -4099,7 +4271,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>203</v>
       </c>
@@ -4113,7 +4285,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>64</v>
       </c>
@@ -4127,7 +4299,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>204</v>
       </c>
@@ -4144,7 +4316,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>205</v>
       </c>
@@ -4158,7 +4330,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>206</v>
       </c>
@@ -4172,7 +4344,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>207</v>
       </c>
@@ -4186,7 +4358,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>208</v>
       </c>
@@ -4203,7 +4375,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>209</v>
       </c>
@@ -4220,7 +4392,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>210</v>
       </c>
@@ -4237,7 +4409,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>211</v>
       </c>
@@ -4254,7 +4426,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>212</v>
       </c>
@@ -4268,7 +4440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>213</v>
       </c>
@@ -4285,7 +4457,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>214</v>
       </c>
@@ -4299,7 +4471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>215</v>
       </c>
@@ -4313,7 +4485,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>216</v>
       </c>
@@ -4327,7 +4499,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>217</v>
       </c>
@@ -4341,7 +4513,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>218</v>
       </c>
@@ -4355,7 +4527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>219</v>
       </c>
@@ -4369,7 +4541,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>220</v>
       </c>
@@ -4383,7 +4555,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>221</v>
       </c>
@@ -4397,7 +4569,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>222</v>
       </c>
@@ -4411,439 +4583,817 @@
         <v>3</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>223</v>
       </c>
+      <c r="B170" t="s">
+        <v>520</v>
+      </c>
       <c r="C170" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D170" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>224</v>
       </c>
+      <c r="B171" t="s">
+        <v>521</v>
+      </c>
       <c r="C171" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D171" t="s">
+        <v>2</v>
+      </c>
+      <c r="E171" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>225</v>
       </c>
+      <c r="B172" t="s">
+        <v>522</v>
+      </c>
       <c r="C172" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D172" t="s">
+        <v>2</v>
+      </c>
+      <c r="E172" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>226</v>
       </c>
+      <c r="B173" t="s">
+        <v>523</v>
+      </c>
       <c r="C173" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D173" t="s">
+        <v>2</v>
+      </c>
+      <c r="E173" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>227</v>
       </c>
+      <c r="B174" t="s">
+        <v>524</v>
+      </c>
       <c r="C174" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D174" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>228</v>
       </c>
+      <c r="B175" t="s">
+        <v>525</v>
+      </c>
       <c r="C175" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D175" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>229</v>
       </c>
+      <c r="B176" t="s">
+        <v>526</v>
+      </c>
       <c r="C176" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D176" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>230</v>
       </c>
+      <c r="B177" t="s">
+        <v>527</v>
+      </c>
       <c r="C177" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D177" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>231</v>
       </c>
+      <c r="B178" t="s">
+        <v>528</v>
+      </c>
       <c r="C178" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D178" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>232</v>
       </c>
+      <c r="B179" t="s">
+        <v>529</v>
+      </c>
       <c r="C179" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D179" t="s">
+        <v>2</v>
+      </c>
+      <c r="E179" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>233</v>
       </c>
+      <c r="B180" t="s">
+        <v>530</v>
+      </c>
       <c r="C180" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D180" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>234</v>
       </c>
+      <c r="B181" t="s">
+        <v>531</v>
+      </c>
       <c r="C181" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D181" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>235</v>
       </c>
+      <c r="B182" t="s">
+        <v>532</v>
+      </c>
       <c r="C182" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D182" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>236</v>
       </c>
+      <c r="B183" t="s">
+        <v>533</v>
+      </c>
       <c r="C183" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D183" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>237</v>
       </c>
+      <c r="B184" t="s">
+        <v>534</v>
+      </c>
       <c r="C184" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D184" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>238</v>
       </c>
+      <c r="B185" t="s">
+        <v>535</v>
+      </c>
       <c r="C185" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D185" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>239</v>
       </c>
+      <c r="B186" t="s">
+        <v>536</v>
+      </c>
       <c r="C186" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D186" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>240</v>
       </c>
+      <c r="B187" t="s">
+        <v>537</v>
+      </c>
       <c r="C187" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D187" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>241</v>
       </c>
+      <c r="B188" t="s">
+        <v>538</v>
+      </c>
       <c r="C188" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D188" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>242</v>
       </c>
+      <c r="B189" t="s">
+        <v>539</v>
+      </c>
       <c r="C189" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D189" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>243</v>
       </c>
+      <c r="B190" t="s">
+        <v>540</v>
+      </c>
       <c r="C190" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D190" t="s">
+        <v>2</v>
+      </c>
+      <c r="E190" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>244</v>
       </c>
+      <c r="B191" t="s">
+        <v>541</v>
+      </c>
       <c r="C191" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D191" t="s">
+        <v>2</v>
+      </c>
+      <c r="E191" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>245</v>
       </c>
+      <c r="B192" t="s">
+        <v>542</v>
+      </c>
       <c r="C192" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D192" t="s">
+        <v>2</v>
+      </c>
+      <c r="E192" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>246</v>
       </c>
+      <c r="B193" t="s">
+        <v>543</v>
+      </c>
       <c r="C193" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D193" t="s">
+        <v>2</v>
+      </c>
+      <c r="E193" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>247</v>
       </c>
+      <c r="B194" t="s">
+        <v>544</v>
+      </c>
       <c r="C194" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D194" t="s">
+        <v>2</v>
+      </c>
+      <c r="E194" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>248</v>
       </c>
+      <c r="B195" t="s">
+        <v>545</v>
+      </c>
       <c r="C195" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D195" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>249</v>
       </c>
+      <c r="B196" t="s">
+        <v>546</v>
+      </c>
       <c r="C196" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D196" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>250</v>
       </c>
+      <c r="B197" t="s">
+        <v>547</v>
+      </c>
       <c r="C197" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D197" t="s">
+        <v>2</v>
+      </c>
+      <c r="E197" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>251</v>
       </c>
+      <c r="B198" t="s">
+        <v>548</v>
+      </c>
       <c r="C198" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D198" t="s">
+        <v>2</v>
+      </c>
+      <c r="E198" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>252</v>
       </c>
+      <c r="B199" t="s">
+        <v>549</v>
+      </c>
       <c r="C199" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D199" t="s">
+        <v>2</v>
+      </c>
+      <c r="E199" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>253</v>
       </c>
+      <c r="B200" t="s">
+        <v>550</v>
+      </c>
       <c r="C200" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D200" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>254</v>
       </c>
+      <c r="B201" t="s">
+        <v>551</v>
+      </c>
       <c r="C201" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D201" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>255</v>
       </c>
+      <c r="B202" t="s">
+        <v>552</v>
+      </c>
       <c r="C202" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D202" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>256</v>
       </c>
+      <c r="B203" t="s">
+        <v>553</v>
+      </c>
       <c r="C203" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D203" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>257</v>
       </c>
+      <c r="B204" t="s">
+        <v>554</v>
+      </c>
       <c r="C204" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D204" t="s">
+        <v>2</v>
+      </c>
+      <c r="E204" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>258</v>
       </c>
+      <c r="B205" t="s">
+        <v>555</v>
+      </c>
       <c r="C205" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D205" t="s">
+        <v>2</v>
+      </c>
+      <c r="E205" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>259</v>
       </c>
+      <c r="B206" t="s">
+        <v>556</v>
+      </c>
       <c r="C206" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D206" t="s">
+        <v>2</v>
+      </c>
+      <c r="E206" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>260</v>
       </c>
+      <c r="B207" t="s">
+        <v>557</v>
+      </c>
       <c r="C207" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D207" t="s">
+        <v>2</v>
+      </c>
+      <c r="E207" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>261</v>
       </c>
+      <c r="B208" t="s">
+        <v>558</v>
+      </c>
       <c r="C208" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D208" t="s">
+        <v>2</v>
+      </c>
+      <c r="E208" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>262</v>
       </c>
+      <c r="B209" t="s">
+        <v>559</v>
+      </c>
       <c r="C209" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D209" t="s">
+        <v>2</v>
+      </c>
+      <c r="E209" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>263</v>
       </c>
+      <c r="B210" t="s">
+        <v>560</v>
+      </c>
       <c r="C210" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D210" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>264</v>
       </c>
+      <c r="B211" t="s">
+        <v>561</v>
+      </c>
       <c r="C211" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D211" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>265</v>
       </c>
+      <c r="B212" t="s">
+        <v>562</v>
+      </c>
       <c r="C212" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D212" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>266</v>
       </c>
+      <c r="B213" t="s">
+        <v>563</v>
+      </c>
       <c r="C213" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D213" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>267</v>
       </c>
+      <c r="B214" t="s">
+        <v>564</v>
+      </c>
       <c r="C214" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D214" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>268</v>
       </c>
+      <c r="B215" t="s">
+        <v>565</v>
+      </c>
       <c r="C215" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D215" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>269</v>
       </c>
+      <c r="B216" t="s">
+        <v>566</v>
+      </c>
       <c r="C216" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D216" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>270</v>
       </c>
+      <c r="B217" t="s">
+        <v>567</v>
+      </c>
       <c r="C217" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D217" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>271</v>
       </c>
+      <c r="B218" t="s">
+        <v>568</v>
+      </c>
       <c r="C218" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D218" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>272</v>
       </c>
+      <c r="B219" t="s">
+        <v>569</v>
+      </c>
       <c r="C219" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D219" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>273</v>
       </c>
+      <c r="B220" t="s">
+        <v>570</v>
+      </c>
       <c r="C220" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D220" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>274</v>
       </c>
+      <c r="B221" t="s">
+        <v>571</v>
+      </c>
       <c r="C221" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D221" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>275</v>
       </c>
+      <c r="B222" t="s">
+        <v>572</v>
+      </c>
       <c r="C222" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D222" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>276</v>
       </c>
+      <c r="B223" t="s">
+        <v>573</v>
+      </c>
       <c r="C223" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D223" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>277</v>
       </c>
@@ -4851,7 +5401,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>278</v>
       </c>
@@ -4859,7 +5409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>279</v>
       </c>
@@ -4867,7 +5417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>280</v>
       </c>
@@ -4875,7 +5425,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>281</v>
       </c>
@@ -4883,7 +5433,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>282</v>
       </c>
@@ -4891,7 +5441,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>283</v>
       </c>
@@ -4899,7 +5449,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>284</v>
       </c>
@@ -4907,7 +5457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>285</v>
       </c>
@@ -4915,7 +5465,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>286</v>
       </c>
@@ -4923,7 +5473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>287</v>
       </c>
@@ -4931,7 +5481,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>288</v>
       </c>
@@ -4939,7 +5489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>289</v>
       </c>
@@ -4947,7 +5497,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>290</v>
       </c>
@@ -4955,7 +5505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>291</v>
       </c>
@@ -4963,7 +5513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>292</v>
       </c>
@@ -4971,7 +5521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>293</v>
       </c>
@@ -4979,7 +5529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>294</v>
       </c>
@@ -4987,7 +5537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>295</v>
       </c>
@@ -4995,7 +5545,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>296</v>
       </c>
@@ -5003,7 +5553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>297</v>
       </c>
@@ -5011,7 +5561,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>298</v>
       </c>
@@ -5019,7 +5569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>299</v>
       </c>
@@ -5027,7 +5577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>300</v>
       </c>
@@ -5035,7 +5585,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>301</v>
       </c>
@@ -5043,7 +5593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>302</v>
       </c>
@@ -5051,7 +5601,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>303</v>
       </c>
@@ -5059,7 +5609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>304</v>
       </c>
@@ -5067,7 +5617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>305</v>
       </c>
@@ -5075,7 +5625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>306</v>
       </c>
@@ -5083,7 +5633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>307</v>
       </c>
@@ -5091,7 +5641,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>308</v>
       </c>
@@ -5099,7 +5649,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>309</v>
       </c>
@@ -5107,7 +5657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>65</v>
       </c>
@@ -5121,7 +5671,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>310</v>
       </c>
@@ -5129,7 +5679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>311</v>
       </c>
@@ -5137,7 +5687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>312</v>
       </c>
@@ -5145,7 +5695,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>313</v>
       </c>
@@ -5153,7 +5703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>66</v>
       </c>
@@ -5167,7 +5717,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>67</v>
       </c>
@@ -5181,7 +5731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>314</v>
       </c>
@@ -5189,7 +5739,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>68</v>
       </c>
@@ -5203,7 +5753,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>315</v>
       </c>
@@ -5211,7 +5761,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>316</v>
       </c>
@@ -5219,7 +5769,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>69</v>
       </c>
@@ -5233,7 +5783,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>70</v>
       </c>
@@ -5244,7 +5794,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>71</v>
       </c>
@@ -5258,7 +5808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>317</v>
       </c>
@@ -5266,7 +5816,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>318</v>
       </c>
@@ -5274,7 +5824,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>319</v>
       </c>
@@ -5282,7 +5832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>320</v>
       </c>
@@ -5290,7 +5840,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>321</v>
       </c>
@@ -5298,7 +5848,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>72</v>
       </c>
@@ -5306,7 +5856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>322</v>
       </c>
@@ -5314,7 +5864,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>323</v>
       </c>
@@ -5322,7 +5872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>324</v>
       </c>
@@ -5330,7 +5880,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>325</v>
       </c>
@@ -5338,7 +5888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>326</v>
       </c>
@@ -5346,7 +5896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>327</v>
       </c>
@@ -5354,7 +5904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>328</v>
       </c>
@@ -5362,7 +5912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>329</v>
       </c>
@@ -5370,7 +5920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
         <v>330</v>
       </c>
@@ -5378,7 +5928,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
         <v>331</v>
       </c>
@@ -5386,7 +5936,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
         <v>332</v>
       </c>
@@ -5394,7 +5944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
         <v>333</v>
       </c>
@@ -5402,7 +5952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
         <v>73</v>
       </c>
@@ -5416,7 +5966,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
         <v>74</v>
       </c>
@@ -5430,7 +5980,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>334</v>
       </c>
@@ -5438,7 +5988,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
         <v>335</v>
       </c>
@@ -5446,7 +5996,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
         <v>336</v>
       </c>
@@ -5454,7 +6004,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
         <v>337</v>
       </c>
@@ -5462,7 +6012,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
         <v>338</v>
       </c>
@@ -5470,7 +6020,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
         <v>339</v>
       </c>
@@ -5478,7 +6028,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
         <v>340</v>
       </c>
@@ -5486,7 +6036,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>341</v>
       </c>
@@ -5494,7 +6044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
         <v>342</v>
       </c>
@@ -5502,7 +6052,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
         <v>343</v>
       </c>
@@ -5510,7 +6060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
         <v>344</v>
       </c>
@@ -5518,7 +6068,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
         <v>345</v>
       </c>
@@ -5526,7 +6076,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
         <v>346</v>
       </c>
@@ -5534,7 +6084,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
         <v>347</v>
       </c>
@@ -5542,7 +6092,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
         <v>348</v>
       </c>
@@ -5550,7 +6100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
         <v>349</v>
       </c>
@@ -5558,7 +6108,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
         <v>350</v>
       </c>
@@ -5566,7 +6116,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
         <v>351</v>
       </c>
@@ -5574,7 +6124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
         <v>352</v>
       </c>
@@ -5582,7 +6132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
         <v>353</v>
       </c>
@@ -5590,7 +6140,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
         <v>354</v>
       </c>
@@ -5598,7 +6148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
         <v>355</v>
       </c>
@@ -5606,7 +6156,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
         <v>356</v>
       </c>
@@ -5614,7 +6164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
         <v>357</v>
       </c>
@@ -5622,7 +6172,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
         <v>358</v>
       </c>
@@ -5630,7 +6180,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
         <v>75</v>
       </c>
@@ -5644,7 +6194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
         <v>359</v>
       </c>
@@ -5652,7 +6202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
         <v>360</v>
       </c>
@@ -5660,7 +6210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
         <v>361</v>
       </c>
@@ -5668,7 +6218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
         <v>362</v>
       </c>
@@ -5676,7 +6226,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
         <v>76</v>
       </c>
@@ -5690,7 +6240,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
         <v>363</v>
       </c>
@@ -5698,7 +6248,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
         <v>364</v>
       </c>
@@ -5706,7 +6256,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
         <v>365</v>
       </c>
@@ -5714,7 +6264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
         <v>366</v>
       </c>
@@ -5722,7 +6272,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
         <v>367</v>
       </c>
@@ -5730,7 +6280,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
         <v>368</v>
       </c>
@@ -5738,7 +6288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
         <v>369</v>
       </c>
@@ -5746,7 +6296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
         <v>370</v>
       </c>
@@ -5754,7 +6304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
         <v>371</v>
       </c>
@@ -5762,7 +6312,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
         <v>372</v>
       </c>
@@ -5779,17 +6329,17 @@
     <mergeCell ref="E76:E80"/>
     <mergeCell ref="B81:B84"/>
     <mergeCell ref="E81:E84"/>
-    <mergeCell ref="B3:B27"/>
-    <mergeCell ref="E3:E27"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="E58:E60"/>
     <mergeCell ref="B85:B90"/>
     <mergeCell ref="E85:E90"/>
     <mergeCell ref="B91:B97"/>
     <mergeCell ref="E91:E97"/>
     <mergeCell ref="B99:B101"/>
     <mergeCell ref="E99:E101"/>
+    <mergeCell ref="B3:B27"/>
+    <mergeCell ref="E3:E27"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="E58:E60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5803,7 +6353,7 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
@@ -5814,7 +6364,7 @@
     <col min="7" max="7" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -5831,7 +6381,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -5854,7 +6404,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -5877,7 +6427,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -5900,7 +6450,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -5923,7 +6473,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -5946,7 +6496,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>44</v>
       </c>
@@ -5966,7 +6516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -5989,7 +6539,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -6012,7 +6562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>47</v>
       </c>
@@ -6032,7 +6582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>77</v>
       </c>
@@ -6055,7 +6605,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>77</v>
       </c>
@@ -6078,7 +6628,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>50</v>
       </c>
@@ -6098,7 +6648,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>51</v>
       </c>
@@ -6118,7 +6668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>52</v>
       </c>
@@ -6138,7 +6688,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>77</v>
       </c>
@@ -6152,7 +6702,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -6169,7 +6719,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>77</v>
       </c>
@@ -6192,7 +6742,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>64</v>
       </c>
@@ -6212,7 +6762,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -6235,7 +6785,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>66</v>
       </c>
@@ -6249,7 +6799,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>67</v>
       </c>
@@ -6269,7 +6819,7 @@
         <v>99999</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -6286,7 +6836,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>69</v>
       </c>
@@ -6306,7 +6856,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>77</v>
       </c>
@@ -6329,7 +6879,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>71</v>
       </c>
@@ -6349,7 +6899,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -6372,7 +6922,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>77</v>
       </c>
@@ -6395,7 +6945,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>77</v>
       </c>
@@ -6418,7 +6968,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>76</v>
       </c>

</xml_diff>